<commit_message>
updated with new test
</commit_message>
<xml_diff>
--- a/code/results/initial_results_testing_rk.xlsx
+++ b/code/results/initial_results_testing_rk.xlsx
@@ -8,24 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\DataScience\Data599\w2020-data599-capstone-projects-ubc-udl\code\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E16D7A-B26F-49D3-A3FB-313E04E8483C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D9ADD5-D329-4A50-AED5-7A855E265FB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19650" yWindow="3825" windowWidth="15375" windowHeight="7095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="2250" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CEC HW Main Meter Power" sheetId="1" r:id="rId1"/>
+    <sheet name="CEC Boiler B-1 Exhaust O2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="33">
   <si>
     <t>Dataset</t>
   </si>
@@ -69,13 +79,73 @@
     <t>- doesn't do this
 - does this
 - does this</t>
+  </si>
+  <si>
+    <t>CEC_compiled_data_5a_updated.csv</t>
+  </si>
+  <si>
+    <t>0.25, 0.33, 0.5, 0.75</t>
+  </si>
+  <si>
+    <t>- Catches almost all human identified anomalies</t>
+  </si>
+  <si>
+    <t>- Catches almost all human identified anomalies
+- Identifies more tp and fp (potentially) than 4 window</t>
+  </si>
+  <si>
+    <t>&lt;2</t>
+  </si>
+  <si>
+    <t>- Catches most large jumps but misses smaller anomalies</t>
+  </si>
+  <si>
+    <t>This was supposed to be 24 hours but clearly messed up the math</t>
+  </si>
+  <si>
+    <t>- Catches most large jumps but misses smaller anomalies
+- Some anomaly windows too long</t>
+  </si>
+  <si>
+    <t>Model Description</t>
+  </si>
+  <si>
+    <t>Pictures</t>
+  </si>
+  <si>
+    <t>data_5a_ts_4_thresh_25_a data_5a_ts_4_thresh_25_b data_5a_ts_4_thresh_33_a data_5a_ts_4_thresh_33_b data_5a_ts_4_thresh_50_a data_5a_ts_4_thresh_50_b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_5a_ts_6_thresh_25_a data_5a_ts_6_thresh_25_b data_5a_ts_6_thresh_33_a data_5a_ts_6_thresh_33_b </t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_5a_ts_32_thresh_25_a data_5a_ts_32_thresh_25_b data_5a_ts_32_thresh_33_a data_5a_ts_32_thresh_33_b </t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_5a_ts_228_thresh_25_a data_5a_ts_228_thresh_25_b data_5a_ts_228_thresh_33_a data_5a_ts_228_thresh_33_b </t>
+  </si>
+  <si>
+    <t>Normal Training Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_5a_norm_ts_4_thresh_25_a data_5a_norm_ts_4_thresh_25_b data_5a_norm_ts_4_thresh_33_a data_5a_norm_ts_4_thresh_33_b </t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_5a_norm_ts_6_thresh_25_a data_5a_norm_ts_6_thresh_25_b data_5a_norm_ts_6_thresh_33_a data_5a_norm_ts_6_thresh_33_b </t>
+  </si>
+  <si>
+    <t>- Similar to non-normal training data
+- Seems to be missing a couple anomalies</t>
+  </si>
+  <si>
+    <t>Model A: [a,b,c] -&gt; mean([a,b,c]): predicts anomaly on c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,6 +157,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -112,11 +188,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -400,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,4 +593,291 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53EB88F0-332F-4F7E-AF47-7B86CFAB5B4F}">
+  <dimension ref="A1:L7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="3">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3">
+        <v>10</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="3">
+        <v>6</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="F3" s="3">
+        <v>10</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="3">
+        <v>32</v>
+      </c>
+      <c r="E4" s="3">
+        <v>8</v>
+      </c>
+      <c r="F4" s="3">
+        <v>10</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="3">
+        <v>228</v>
+      </c>
+      <c r="E5" s="3">
+        <v>57</v>
+      </c>
+      <c r="F5" s="3">
+        <v>10</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="3">
+        <v>4</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
+        <v>10</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="3">
+        <v>6</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="F7" s="3">
+        <v>10</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated with new models
</commit_message>
<xml_diff>
--- a/code/results/initial_results_testing_rk.xlsx
+++ b/code/results/initial_results_testing_rk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\DataScience\Data599\w2020-data599-capstone-projects-ubc-udl\code\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D9ADD5-D329-4A50-AED5-7A855E265FB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B11F0C-16B7-4903-8CC1-2869B0FEE201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="2250" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CEC HW Main Meter Power" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="50">
   <si>
     <t>Dataset</t>
   </si>
@@ -87,9 +87,6 @@
     <t>0.25, 0.33, 0.5, 0.75</t>
   </si>
   <si>
-    <t>- Catches almost all human identified anomalies</t>
-  </si>
-  <si>
     <t>- Catches almost all human identified anomalies
 - Identifies more tp and fp (potentially) than 4 window</t>
   </si>
@@ -138,7 +135,66 @@
 - Seems to be missing a couple anomalies</t>
   </si>
   <si>
-    <t>Model A: [a,b,c] -&gt; mean([a,b,c]): predicts anomaly on c</t>
+    <t>Model C: Train [a,b,c] -&gt; c: predicts anomaly on mean([a,b,c])</t>
+  </si>
+  <si>
+    <t>Model A: Train [a,b,c] -&gt; d: predicts anomaly on d</t>
+  </si>
+  <si>
+    <t>Model B: [a,b,c] -&gt; [a,b,c]: predicts anomaly on mean([a,b,c])</t>
+  </si>
+  <si>
+    <t>No significant difference from all data</t>
+  </si>
+  <si>
+    <t>0.25, 0.5, 0.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_5a_PD_ts_4_thresh_25_a data_5a_PD_ts_4_thresh_25_b data_5a_PD_ts_4_thresh_25_c data_5a_PD_ts_4_thresh_50_a data_5a_PD_ts_4_thresh_50_b  data_5a_PD_ts_4_thresh_75_a </t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_5a_PD_ts_8_thresh_25_a data_5a_PD_ts_8_thresh_25_b data_5a_PD_ts_8_thresh_25_c data_5a_PD_ts_8_thresh_50_a data_5a_PD_ts_8_thresh_50_b  data_5a_PD_ts_8_thresh_75_a </t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_5a_PD_ts_48_thresh_25_a data_5a_PD_ts_48_thresh_25_b data_5a_PD_ts_48_thresh_25_c data_5a_PD_ts_48_thresh_50_a   data_5a_PD_ts_48_thresh_75_a </t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_5a_PD_ts_4_thresh_25_a data_5a_PD_ts_4_thresh_25_b data_5a_PD_ts_8_thresh_25_c </t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_5a_PD_ts_8_thresh_25_a data_5a_PD_ts_8_thresh_25_b data_5a_PD_ts_8_thresh_25_c  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_5a_SW_ts_4_thresh_25_a data_5a_SW_ts_4_thresh_25_b data_5a_SW_ts_4_thresh_25_c data_5a_SW_ts_4_thresh_50_a data_5a_SW_ts_4_thresh_50_b  data_5a_SW_ts_4_thresh_75_a </t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_5a_SW_ts_8_thresh_25_a data_5a_SW_ts_8_thresh_25_b data_5a_SW_ts_8_thresh_25_c data_5a_SW_ts_8_thresh_50_a data_5a_SW_ts_8_thresh_50_b  data_5a_SW_ts_8_thresh_75_a </t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_5a_SW_ts_48_thresh_25_a data_5a_SW_ts_48_thresh_25_b data_5a_SW_ts_48_thresh_25_c data_5a_SW_ts_48_thresh_50_a   data_5a_SW_ts_48_thresh_75_a </t>
+  </si>
+  <si>
+    <t>- Catches most jump anomalies
+- Short window prevents from anomalies from dragging on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Catches most jump anomalies (couple less than 4 window)
+</t>
+  </si>
+  <si>
+    <t>- Catches most jump anomalies (couple less than 4 window)
+- PD prediction in general prevents anomalies from dragging on</t>
+  </si>
+  <si>
+    <t>- Very little difference from non-normal data</t>
+  </si>
+  <si>
+    <t>- Catches more contextual anomalies. Misses a couple jumps (more than 4)
+- Longer window starts dragging on anomalies</t>
+  </si>
+  <si>
+    <t>- Misses quite a few anomlies
+- Longer window starts drags in long sequences</t>
   </si>
 </sst>
 </file>
@@ -188,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
@@ -208,6 +264,12 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -597,10 +659,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53EB88F0-332F-4F7E-AF47-7B86CFAB5B4F}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,7 +689,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -654,10 +716,10 @@
         <v>9</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -667,30 +729,30 @@
       <c r="C2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="8">
         <v>4</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="8">
         <v>1</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="8">
         <v>10</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="3">
+        <v>17</v>
+      </c>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="8">
         <v>0.25</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="90" x14ac:dyDescent="0.25">
@@ -703,33 +765,33 @@
       <c r="C3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="3">
-        <v>6</v>
-      </c>
-      <c r="E3" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="F3" s="3">
+      <c r="D3" s="8">
+        <v>8</v>
+      </c>
+      <c r="E3" s="8">
+        <v>2</v>
+      </c>
+      <c r="F3" s="8">
         <v>10</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="3">
+        <v>17</v>
+      </c>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="8">
         <v>0.25</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
@@ -739,140 +801,432 @@
       <c r="C4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="3">
-        <v>32</v>
-      </c>
-      <c r="E4" s="3">
-        <v>8</v>
-      </c>
-      <c r="F4" s="3">
+      <c r="D4" s="8">
+        <v>48</v>
+      </c>
+      <c r="E4" s="8">
+        <v>12</v>
+      </c>
+      <c r="F4" s="8">
         <v>10</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="3">
+        <v>17</v>
+      </c>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="8">
         <v>0.25</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="3">
-        <v>228</v>
-      </c>
-      <c r="E5" s="3">
-        <v>57</v>
-      </c>
-      <c r="F5" s="3">
+      <c r="D5" s="8">
+        <v>4</v>
+      </c>
+      <c r="E5" s="8">
+        <v>1</v>
+      </c>
+      <c r="F5" s="8">
         <v>10</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="3">
+        <v>17</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="8">
         <v>0.25</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="L5" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="8">
+        <v>8</v>
+      </c>
+      <c r="E6" s="8">
+        <v>2</v>
+      </c>
+      <c r="F6" s="8">
+        <v>10</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="8">
         <v>4</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E7" s="8">
         <v>1</v>
       </c>
-      <c r="F6" s="3">
-        <v>10</v>
-      </c>
-      <c r="G6" s="7" t="s">
+      <c r="F7" s="8">
+        <v>10</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="8">
+        <v>8</v>
+      </c>
+      <c r="E8" s="8">
+        <v>2</v>
+      </c>
+      <c r="F8" s="8">
+        <v>10</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="8">
+        <v>48</v>
+      </c>
+      <c r="E9" s="8">
+        <v>12</v>
+      </c>
+      <c r="F9" s="8">
+        <v>10</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J9" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="3">
+        <v>4</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3">
+        <v>10</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="3">
+        <v>6</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="F11" s="3">
+        <v>10</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="3">
+        <v>32</v>
+      </c>
+      <c r="E12" s="3">
+        <v>8</v>
+      </c>
+      <c r="F12" s="3">
+        <v>10</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="K12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3" t="s">
+      <c r="L12" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="3">
+        <v>228</v>
+      </c>
+      <c r="E13" s="3">
+        <v>57</v>
+      </c>
+      <c r="F13" s="3">
+        <v>10</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="K6" s="5" t="s">
+      <c r="J13" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="D14" s="3">
+        <v>4</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3">
+        <v>10</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="3">
+        <v>6</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="F15" s="3">
+        <v>10</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L15" s="6" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="3">
-        <v>6</v>
-      </c>
-      <c r="E7" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="F7" s="3">
-        <v>10</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>